<commit_message>
More SQL keywords to functions.xlsx
</commit_message>
<xml_diff>
--- a/references/functions.xlsx
+++ b/references/functions.xlsx
@@ -12,7 +12,7 @@
     <sheet state="visible" name="regex" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">cli!$A$1:$F$1022</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">cli!$A$1:$F$1023</definedName>
     <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">python!$D$1:$D$1002</definedName>
     <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">sql!$D$1:$D$1003</definedName>
     <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">os!$D$1:$D$1003</definedName>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="625">
   <si>
     <t>1. Text that needs to be replaced will be surrounded by &lt; &gt;
 2. In the case that angle brackets is part of the syntax, the following characters will be used in descending priority...&lt; &gt;
@@ -115,6 +115,9 @@
     <t>Syntax</t>
   </si>
   <si>
+    <t>Metadata</t>
+  </si>
+  <si>
     <t>&lt;entity&gt;_&lt;verb&gt;_&lt;id&gt;</t>
   </si>
   <si>
@@ -711,6 +714,16 @@
   </si>
   <si>
     <t>1. creates branch and switches to that branch</t>
+  </si>
+  <si>
+    <t>commit-amend_1</t>
+  </si>
+  <si>
+    <t>git commit --amend -m '&lt;message&gt;'</t>
+  </si>
+  <si>
+    <t>notes:
+  1: "Amends most recent commit message"</t>
   </si>
   <si>
     <t>config_1</t>
@@ -1786,6 +1799,20 @@
   </si>
   <si>
     <t>distinct_1</t>
+  </si>
+  <si>
+    <t>union_1</t>
+  </si>
+  <si>
+    <t>Notes:
+  1: "Does deduplicate.  Union all does not deduplicate"</t>
+  </si>
+  <si>
+    <t>union-all_1</t>
+  </si>
+  <si>
+    <t>Notes:
+  1: "Does not deduplicate.  Union does deduplicate"</t>
   </si>
   <si>
     <t>file_rename_1</t>
@@ -2261,7 +2288,7 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2303,32 +2330,32 @@
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -10995,1177 +11022,1175 @@
         <v>5</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" hidden="1">
       <c r="A2" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
       <c r="E2" s="25"/>
       <c r="F2" s="24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" hidden="1">
       <c r="A3" s="26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
     </row>
     <row r="4" hidden="1">
       <c r="A4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
     </row>
     <row r="5" hidden="1">
       <c r="A5" s="26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
     </row>
     <row r="6" hidden="1">
       <c r="A6" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" hidden="1">
       <c r="A7" s="26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" hidden="1">
       <c r="A8" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" hidden="1">
       <c r="A9" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="27"/>
     </row>
     <row r="10" hidden="1">
       <c r="A10" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" ht="20.25" hidden="1" customHeight="1">
       <c r="A11" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" ht="235.5" hidden="1" customHeight="1">
       <c r="A12" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" hidden="1">
       <c r="A13" s="26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" hidden="1">
       <c r="A14" s="28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
     </row>
     <row r="15" hidden="1">
       <c r="A15" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" hidden="1">
       <c r="A16" s="28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
     </row>
     <row r="17" hidden="1">
       <c r="A17" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>68</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>67</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
     </row>
     <row r="18" hidden="1">
       <c r="A18" s="28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
     </row>
     <row r="19" hidden="1">
       <c r="A19" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" hidden="1">
       <c r="A20" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
     </row>
     <row r="21" hidden="1">
       <c r="A21" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
     </row>
     <row r="22" hidden="1">
       <c r="A22" s="28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" hidden="1">
       <c r="A23" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
     </row>
     <row r="24" hidden="1">
       <c r="A24" s="28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" hidden="1">
       <c r="A25" s="26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" hidden="1">
       <c r="A26" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
     </row>
     <row r="27" hidden="1">
       <c r="A27" s="26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" hidden="1">
       <c r="A28" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" hidden="1">
       <c r="A29" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" hidden="1">
       <c r="A30" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E30" s="29"/>
       <c r="F30" s="28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" hidden="1">
       <c r="A31" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" hidden="1">
       <c r="A32" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" hidden="1">
       <c r="A33" s="26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C33" s="27"/>
       <c r="D33" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" hidden="1">
       <c r="A34" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
     </row>
     <row r="35" hidden="1">
       <c r="A35" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
     </row>
     <row r="36" hidden="1">
       <c r="A36" s="28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
     </row>
     <row r="37" hidden="1">
       <c r="A37" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
     </row>
     <row r="38" hidden="1">
       <c r="A38" s="28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
     </row>
     <row r="39" hidden="1">
       <c r="A39" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C39" s="27"/>
       <c r="D39" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" hidden="1">
       <c r="A40" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C40" s="29"/>
       <c r="D40" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
     </row>
     <row r="41" hidden="1">
       <c r="A41" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
     </row>
     <row r="42" hidden="1">
       <c r="A42" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
     </row>
     <row r="43" hidden="1">
       <c r="A43" s="26" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C43" s="27"/>
       <c r="D43" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
     </row>
     <row r="44" hidden="1">
       <c r="A44" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" hidden="1">
       <c r="A45" s="26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" hidden="1">
       <c r="A46" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C46" s="29"/>
       <c r="D46" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E46" s="29"/>
       <c r="F46" s="29"/>
     </row>
     <row r="47" hidden="1">
       <c r="A47" s="26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="27"/>
     </row>
     <row r="48" hidden="1">
       <c r="A48" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C48" s="29"/>
       <c r="D48" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
     </row>
     <row r="49" hidden="1">
       <c r="A49" s="26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49" s="32"/>
     </row>
     <row r="50" hidden="1">
       <c r="A50" s="28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C50" s="29"/>
       <c r="D50" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E50" s="29"/>
       <c r="F50" s="28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" hidden="1">
       <c r="A51" s="26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C51" s="27"/>
       <c r="D51" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51" s="26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" hidden="1">
       <c r="A52" s="28" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C52" s="29"/>
       <c r="D52" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E52" s="29"/>
       <c r="F52" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" hidden="1">
       <c r="A53" s="26" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C53" s="27"/>
       <c r="D53" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
     </row>
     <row r="54" hidden="1">
       <c r="A54" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C54" s="29"/>
       <c r="D54" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E54" s="29"/>
       <c r="F54" s="29"/>
     </row>
     <row r="55" hidden="1">
       <c r="A55" s="26" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C55" s="32"/>
       <c r="D55" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="26"/>
     </row>
     <row r="56" hidden="1">
       <c r="A56" s="28" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B56" s="28"/>
       <c r="C56" s="28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" hidden="1">
       <c r="A57" s="26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57" s="27"/>
     </row>
     <row r="58" hidden="1">
       <c r="A58" s="28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E58" s="29"/>
       <c r="F58" s="29"/>
     </row>
     <row r="59" hidden="1">
       <c r="A59" s="26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B59" s="27"/>
       <c r="C59" s="26" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59" s="26" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" hidden="1">
       <c r="A60" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C60" s="29"/>
       <c r="D60" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="29"/>
     </row>
     <row r="61" hidden="1">
       <c r="A61" s="26" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E61" s="27"/>
       <c r="F61" s="26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" hidden="1">
       <c r="A62" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="29"/>
     </row>
     <row r="63" hidden="1">
       <c r="A63" s="26" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B63" s="27"/>
       <c r="C63" s="26" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E63" s="27"/>
       <c r="F63" s="26" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" hidden="1">
       <c r="A64" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B64" s="29"/>
       <c r="C64" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E64" s="29"/>
       <c r="F64" s="28" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" hidden="1">
       <c r="A65" s="26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E65" s="27"/>
       <c r="F65" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" hidden="1">
       <c r="A66" s="28" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C67" s="26"/>
       <c r="D67" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E67" s="27"/>
       <c r="F67" s="33" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C68" s="29"/>
       <c r="D68" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E68" s="29"/>
       <c r="F68" s="34"/>
     </row>
     <row r="69">
       <c r="A69" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E69" s="27"/>
       <c r="F69" s="33" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E70" s="29"/>
       <c r="F70" s="34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35" t="s">
+      <c r="A71" s="26" t="s">
         <v>217</v>
       </c>
+      <c r="B71" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C71" s="26"/>
       <c r="D71" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E71" s="36"/>
-      <c r="F71" s="37"/>
+        <v>205</v>
+      </c>
+      <c r="E71" s="27"/>
+      <c r="F71" s="33" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="B72" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="C72" s="28" t="s">
+      <c r="A72" s="22" t="s">
         <v>220</v>
       </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22" t="s">
+        <v>221</v>
+      </c>
       <c r="D72" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="E72" s="29"/>
-      <c r="F72" s="34"/>
+        <v>205</v>
+      </c>
+      <c r="E72" s="25"/>
+      <c r="F72" s="35"/>
     </row>
     <row r="73">
       <c r="A73" s="26" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="C73" s="32" t="s">
         <v>223</v>
       </c>
+      <c r="C73" s="26" t="s">
+        <v>224</v>
+      </c>
       <c r="D73" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E73" s="27"/>
       <c r="F73" s="33"/>
     </row>
     <row r="74">
       <c r="A74" s="28" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="29"/>
+        <v>226</v>
+      </c>
+      <c r="C74" s="36" t="s">
+        <v>227</v>
+      </c>
       <c r="D74" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E74" s="29"/>
-      <c r="F74" s="34" t="s">
-        <v>226</v>
-      </c>
+      <c r="F74" s="34"/>
     </row>
     <row r="75">
       <c r="A75" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C75" s="26"/>
+        <v>229</v>
+      </c>
+      <c r="C75" s="27"/>
       <c r="D75" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E75" s="27"/>
       <c r="F75" s="33" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="28" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="C76" s="28" t="s">
         <v>232</v>
       </c>
+      <c r="C76" s="28"/>
       <c r="D76" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E76" s="29"/>
       <c r="F76" s="34" t="s">
@@ -12179,291 +12204,291 @@
       <c r="B77" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="C77" s="26"/>
+      <c r="C77" s="26" t="s">
+        <v>236</v>
+      </c>
       <c r="D77" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E77" s="27"/>
       <c r="F77" s="33" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" hidden="1">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78">
       <c r="A78" s="28" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="C78" s="29"/>
+        <v>239</v>
+      </c>
+      <c r="C78" s="28"/>
       <c r="D78" s="28" t="s">
-        <v>35</v>
+        <v>205</v>
       </c>
       <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
+      <c r="F78" s="34" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="79" hidden="1">
       <c r="A79" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C79" s="27"/>
       <c r="D79" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E79" s="27"/>
-      <c r="F79" s="26" t="s">
-        <v>241</v>
-      </c>
+      <c r="F79" s="27"/>
     </row>
     <row r="80" hidden="1">
       <c r="A80" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="B80" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="C80" s="30" t="s">
+      <c r="B80" s="28" t="s">
         <v>244</v>
       </c>
+      <c r="C80" s="29"/>
       <c r="D80" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
+      <c r="F80" s="28" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="81" hidden="1">
       <c r="A81" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="B81" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="B81" s="31" t="s">
         <v>247</v>
       </c>
+      <c r="C81" s="31" t="s">
+        <v>248</v>
+      </c>
       <c r="D81" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E81" s="27"/>
-      <c r="F81" s="26" t="s">
-        <v>248</v>
-      </c>
+      <c r="F81" s="27"/>
     </row>
     <row r="82" hidden="1">
       <c r="A82" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="B82" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="C82" s="28" t="s">
+      <c r="B82" s="14" t="s">
         <v>250</v>
       </c>
+      <c r="C82" s="14" t="s">
+        <v>251</v>
+      </c>
       <c r="D82" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E82" s="29"/>
       <c r="F82" s="28" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" hidden="1">
       <c r="A83" s="26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="C83" s="27"/>
+        <v>250</v>
+      </c>
+      <c r="C83" s="26" t="s">
+        <v>254</v>
+      </c>
       <c r="D83" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
+      <c r="F83" s="26" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="84" hidden="1">
       <c r="A84" s="28" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C84" s="29"/>
       <c r="D84" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E84" s="29"/>
       <c r="F84" s="29"/>
     </row>
     <row r="85" hidden="1">
       <c r="A85" s="26" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="C85" s="26" t="s">
-        <v>258</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C85" s="27"/>
       <c r="D85" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E85" s="27"/>
-      <c r="F85" s="26" t="s">
-        <v>259</v>
-      </c>
+      <c r="F85" s="27"/>
     </row>
     <row r="86" hidden="1">
       <c r="A86" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="B86" s="29"/>
+      <c r="B86" s="28" t="s">
+        <v>261</v>
+      </c>
       <c r="C86" s="28" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E86" s="29"/>
       <c r="F86" s="28" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" hidden="1">
       <c r="A87" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="B87" s="26" t="s">
         <v>264</v>
       </c>
+      <c r="B87" s="27"/>
       <c r="C87" s="26" t="s">
         <v>265</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
+      <c r="F87" s="26" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="88" hidden="1">
       <c r="A88" s="28" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
     </row>
     <row r="89" hidden="1">
       <c r="A89" s="26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="C89" s="27"/>
+        <v>271</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>272</v>
+      </c>
       <c r="D89" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E89" s="27"/>
-      <c r="F89" s="26" t="s">
-        <v>271</v>
-      </c>
+      <c r="F89" s="27"/>
     </row>
     <row r="90" hidden="1">
       <c r="A90" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="28" t="s">
         <v>273</v>
       </c>
+      <c r="B90" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C90" s="29"/>
       <c r="D90" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
+      <c r="F90" s="28" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="91" hidden="1">
       <c r="A91" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="B91" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="C91" s="27"/>
+        <v>276</v>
+      </c>
+      <c r="B91" s="27"/>
+      <c r="C91" s="26" t="s">
+        <v>277</v>
+      </c>
       <c r="D91" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E91" s="27"/>
       <c r="F91" s="27"/>
     </row>
     <row r="92" hidden="1">
       <c r="A92" s="28" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C92" s="29"/>
       <c r="D92" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E92" s="29"/>
       <c r="F92" s="29"/>
     </row>
     <row r="93" hidden="1">
       <c r="A93" s="26" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C93" s="27"/>
       <c r="D93" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E93" s="27"/>
       <c r="F93" s="27"/>
     </row>
     <row r="94" hidden="1">
       <c r="A94" s="28" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C94" s="29"/>
       <c r="D94" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E94" s="29"/>
-      <c r="F94" s="28" t="s">
-        <v>282</v>
-      </c>
+      <c r="F94" s="29"/>
     </row>
     <row r="95" hidden="1">
       <c r="A95" s="26" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="C95" s="38" t="s">
         <v>285</v>
       </c>
+      <c r="C95" s="27"/>
       <c r="D95" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E95" s="27"/>
       <c r="F95" s="26" t="s">
@@ -12477,156 +12502,156 @@
       <c r="B96" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="C96" s="29"/>
+      <c r="C96" s="37" t="s">
+        <v>289</v>
+      </c>
       <c r="D96" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E96" s="29"/>
       <c r="F96" s="28" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" hidden="1">
       <c r="A97" s="26" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="C97" s="32" t="s">
         <v>292</v>
       </c>
+      <c r="C97" s="27"/>
       <c r="D97" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
+      <c r="F97" s="26" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="98" hidden="1">
       <c r="A98" s="28" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="C98" s="29"/>
+        <v>295</v>
+      </c>
+      <c r="C98" s="36" t="s">
+        <v>296</v>
+      </c>
       <c r="D98" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E98" s="29"/>
       <c r="F98" s="29"/>
     </row>
     <row r="99" hidden="1">
       <c r="A99" s="26" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C99" s="27"/>
       <c r="D99" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E99" s="27"/>
-      <c r="F99" s="26" t="s">
-        <v>297</v>
-      </c>
+      <c r="F99" s="27"/>
     </row>
     <row r="100" hidden="1">
       <c r="A100" s="28" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C100" s="29"/>
       <c r="D100" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E100" s="29"/>
       <c r="F100" s="28" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="101" hidden="1">
       <c r="A101" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C101" s="27"/>
       <c r="D101" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E101" s="27"/>
       <c r="F101" s="26" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="102" hidden="1">
       <c r="A102" s="28" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C102" s="29"/>
       <c r="D102" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E102" s="29"/>
       <c r="F102" s="28" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" hidden="1">
       <c r="A103" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C103" s="27"/>
       <c r="D103" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E103" s="27"/>
       <c r="F103" s="26" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" hidden="1">
       <c r="A104" s="28" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C104" s="29"/>
       <c r="D104" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
+      <c r="F104" s="28" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="105" hidden="1">
       <c r="A105" s="26" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="C105" s="26" t="s">
-        <v>314</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="C105" s="27"/>
       <c r="D105" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E105" s="27"/>
-      <c r="F105" s="26" t="s">
-        <v>315</v>
-      </c>
+      <c r="F105" s="27"/>
     </row>
     <row r="106" hidden="1">
       <c r="A106" s="28" t="s">
@@ -12635,136 +12660,136 @@
       <c r="B106" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="C106" s="29"/>
+      <c r="C106" s="28" t="s">
+        <v>318</v>
+      </c>
       <c r="D106" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E106" s="29"/>
       <c r="F106" s="28" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="107" hidden="1">
       <c r="A107" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
+      <c r="F107" s="26" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="108" hidden="1">
       <c r="A108" s="28" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C108" s="29"/>
       <c r="D108" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E108" s="29"/>
-      <c r="F108" s="28" t="s">
-        <v>323</v>
-      </c>
+      <c r="F108" s="29"/>
     </row>
     <row r="109" hidden="1">
       <c r="A109" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C109" s="27"/>
       <c r="D109" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
+      <c r="F109" s="26" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="110" hidden="1">
       <c r="A110" s="28" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C110" s="29"/>
       <c r="D110" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E110" s="29"/>
       <c r="F110" s="29"/>
     </row>
     <row r="111" hidden="1">
       <c r="A111" s="26" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>329</v>
-      </c>
-      <c r="C111" s="32"/>
+        <v>331</v>
+      </c>
+      <c r="C111" s="27"/>
       <c r="D111" s="26" t="s">
-        <v>330</v>
+        <v>36</v>
       </c>
       <c r="E111" s="27"/>
       <c r="F111" s="27"/>
     </row>
     <row r="112" hidden="1">
       <c r="A112" s="28" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="C112" s="30" t="s">
         <v>333</v>
       </c>
+      <c r="C112" s="36"/>
       <c r="D112" s="28" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E112" s="29"/>
-      <c r="F112" s="28" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="113">
+      <c r="F112" s="29"/>
+    </row>
+    <row r="113" hidden="1">
       <c r="A113" s="26" t="s">
         <v>335</v>
       </c>
       <c r="B113" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="C113" s="27"/>
+      <c r="C113" s="31" t="s">
+        <v>337</v>
+      </c>
       <c r="D113" s="26" t="s">
-        <v>204</v>
+        <v>334</v>
       </c>
       <c r="E113" s="27"/>
-      <c r="F113" s="39"/>
+      <c r="F113" s="26" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="28" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>338</v>
-      </c>
-      <c r="C114" s="28" t="s">
-        <v>339</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="C114" s="29"/>
       <c r="D114" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E114" s="29"/>
-      <c r="F114" s="34" t="s">
-        <v>340</v>
-      </c>
+      <c r="F114" s="38"/>
     </row>
     <row r="115">
       <c r="A115" s="26" t="s">
@@ -12773,43 +12798,43 @@
       <c r="B115" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="C115" s="27"/>
+      <c r="C115" s="26" t="s">
+        <v>343</v>
+      </c>
       <c r="D115" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E115" s="27"/>
       <c r="F115" s="33" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="28" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C116" s="29"/>
       <c r="D116" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E116" s="29"/>
       <c r="F116" s="34" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="26" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="C117" s="26" t="s">
         <v>349</v>
       </c>
+      <c r="C117" s="27"/>
       <c r="D117" s="26" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E117" s="27"/>
       <c r="F117" s="33" t="s">
@@ -12823,118 +12848,120 @@
       <c r="B118" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="C118" s="29"/>
-      <c r="D118" s="28"/>
+      <c r="C118" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="D118" s="28" t="s">
+        <v>205</v>
+      </c>
       <c r="E118" s="29"/>
       <c r="F118" s="34" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="35" t="s">
-        <v>354</v>
-      </c>
-      <c r="B119" s="35" t="s">
+      <c r="A119" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="C119" s="40"/>
-      <c r="D119" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E119" s="36"/>
-      <c r="F119" s="41" t="s">
+      <c r="B119" s="26" t="s">
         <v>356</v>
+      </c>
+      <c r="C119" s="27"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="33" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="22" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C120" s="23"/>
       <c r="D120" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E120" s="25"/>
-      <c r="F120" s="22"/>
+      <c r="F120" s="39" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" s="35" t="s">
-        <v>359</v>
-      </c>
-      <c r="B121" s="35" t="s">
-        <v>360</v>
-      </c>
-      <c r="C121" s="40"/>
+      <c r="A121" s="40" t="s">
+        <v>361</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="C121" s="41"/>
       <c r="D121" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E121" s="36"/>
-      <c r="F121" s="35"/>
+        <v>205</v>
+      </c>
+      <c r="E121" s="42"/>
+      <c r="F121" s="40"/>
     </row>
     <row r="122">
       <c r="A122" s="22" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C122" s="23"/>
       <c r="D122" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E122" s="25"/>
-      <c r="F122" s="22" t="s">
-        <v>363</v>
-      </c>
+      <c r="F122" s="22"/>
     </row>
     <row r="123">
-      <c r="A123" s="35" t="s">
-        <v>364</v>
-      </c>
-      <c r="B123" s="35"/>
-      <c r="C123" s="40" t="s">
+      <c r="A123" s="40" t="s">
         <v>365</v>
       </c>
+      <c r="B123" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="C123" s="41"/>
       <c r="D123" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E123" s="36"/>
-      <c r="F123" s="35" t="s">
-        <v>366</v>
+        <v>205</v>
+      </c>
+      <c r="E123" s="42"/>
+      <c r="F123" s="40" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="B124" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="C124" s="23"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="23" t="s">
+        <v>369</v>
+      </c>
       <c r="D124" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E124" s="25"/>
-      <c r="F124" s="22"/>
-    </row>
-    <row r="125" hidden="1">
-      <c r="A125" s="26" t="s">
-        <v>369</v>
-      </c>
-      <c r="B125" s="26" t="s">
+      <c r="F124" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="C125" s="32" t="s">
+    </row>
+    <row r="125">
+      <c r="A125" s="40" t="s">
         <v>371</v>
       </c>
+      <c r="B125" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="C125" s="41"/>
       <c r="D125" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="E125" s="27"/>
-      <c r="F125" s="27"/>
+        <v>205</v>
+      </c>
+      <c r="E125" s="42"/>
+      <c r="F125" s="40"/>
     </row>
     <row r="126" hidden="1">
       <c r="A126" s="28" t="s">
@@ -12943,7 +12970,7 @@
       <c r="B126" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="C126" s="28" t="s">
+      <c r="C126" s="36" t="s">
         <v>375</v>
       </c>
       <c r="D126" s="28" t="s">
@@ -12953,18 +12980,24 @@
       <c r="F126" s="29"/>
     </row>
     <row r="127" hidden="1">
-      <c r="A127" s="27"/>
-      <c r="B127" s="27"/>
-      <c r="C127" s="27"/>
-      <c r="D127" s="27"/>
+      <c r="A127" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="B127" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D127" s="26" t="s">
+        <v>380</v>
+      </c>
       <c r="E127" s="27"/>
       <c r="F127" s="27"/>
     </row>
     <row r="128" hidden="1">
       <c r="A128" s="29"/>
-      <c r="B128" s="28" t="s">
-        <v>247</v>
-      </c>
+      <c r="B128" s="29"/>
       <c r="C128" s="29"/>
       <c r="D128" s="29"/>
       <c r="E128" s="29"/>
@@ -12972,7 +13005,9 @@
     </row>
     <row r="129" hidden="1">
       <c r="A129" s="27"/>
-      <c r="B129" s="27"/>
+      <c r="B129" s="26" t="s">
+        <v>251</v>
+      </c>
       <c r="C129" s="27"/>
       <c r="D129" s="27"/>
       <c r="E129" s="27"/>
@@ -20122,8 +20157,16 @@
       <c r="E1022" s="29"/>
       <c r="F1022" s="29"/>
     </row>
+    <row r="1023" hidden="1">
+      <c r="A1023" s="27"/>
+      <c r="B1023" s="27"/>
+      <c r="C1023" s="27"/>
+      <c r="D1023" s="27"/>
+      <c r="E1023" s="27"/>
+      <c r="F1023" s="27"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$1022">
+  <autoFilter ref="$A$1:$F$1023">
     <filterColumn colId="3">
       <filters>
         <filter val="git"/>
@@ -20158,241 +20201,241 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>377</v>
-      </c>
-      <c r="F1" s="42" t="s">
+      <c r="E1" s="43" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="43" t="s">
-        <v>23</v>
+      <c r="A2" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
-      <c r="F2" s="43" t="s">
-        <v>24</v>
+      <c r="F2" s="39" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="46" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E3" s="48"/>
       <c r="F3" s="49" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="50" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="51" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
     <row r="5">
       <c r="A5" s="46" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="47" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="47" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="50" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C6" s="52"/>
       <c r="D6" s="51" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52"/>
     </row>
     <row r="7">
       <c r="A7" s="46" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="47" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="50" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
     </row>
     <row r="9">
       <c r="A9" s="46" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="47" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="47" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="50" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C10" s="52"/>
       <c r="D10" s="51" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E10" s="52"/>
       <c r="F10" s="51" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="46" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="47" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="47" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="50" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E12" s="52"/>
       <c r="F12" s="51" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="46" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="47" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48"/>
     </row>
     <row r="14">
       <c r="A14" s="50" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="50" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
     </row>
     <row r="15">
       <c r="A15" s="46" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
       <c r="F15" s="46" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16">
@@ -28334,108 +28377,108 @@
         <v>4</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>417</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>6</v>
+        <v>421</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="G2" s="25"/>
     </row>
     <row r="3" hidden="1">
       <c r="A3" s="53" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
       <c r="D3" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E3" s="53"/>
       <c r="F3" s="53" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="G3" s="54"/>
     </row>
     <row r="4" hidden="1">
       <c r="A4" s="55" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C4" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" s="56" t="s">
         <v>424</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>420</v>
       </c>
       <c r="E4" s="56"/>
       <c r="F4" s="56" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="G4" s="57"/>
     </row>
     <row r="5">
       <c r="A5" s="53" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="F5" s="53"/>
       <c r="G5" s="54"/>
     </row>
     <row r="6">
       <c r="A6" s="56" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="B6" s="56"/>
       <c r="C6" s="57"/>
       <c r="D6" s="56" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G6" s="57"/>
     </row>
     <row r="7" hidden="1">
       <c r="A7" s="53" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="53" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="49"/>
@@ -28443,14 +28486,14 @@
     </row>
     <row r="8" hidden="1">
       <c r="A8" s="56" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B8" s="58"/>
       <c r="C8" s="56" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E8" s="56"/>
       <c r="F8" s="58"/>
@@ -28458,16 +28501,16 @@
     </row>
     <row r="9" hidden="1">
       <c r="A9" s="53" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E9" s="53"/>
       <c r="F9" s="49"/>
@@ -28475,14 +28518,14 @@
     </row>
     <row r="10" hidden="1">
       <c r="A10" s="56" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C10" s="58"/>
       <c r="D10" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E10" s="56"/>
       <c r="F10" s="57"/>
@@ -28490,181 +28533,181 @@
     </row>
     <row r="11" hidden="1">
       <c r="A11" s="53" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="53" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="G11" s="54"/>
     </row>
     <row r="12" hidden="1">
       <c r="A12" s="56" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D12" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E12" s="56"/>
       <c r="F12" s="56" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="G12" s="57"/>
     </row>
     <row r="13" hidden="1">
       <c r="A13" s="53" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="53" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="G13" s="54"/>
     </row>
     <row r="14" hidden="1">
       <c r="A14" s="56" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="56" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="G14" s="57"/>
     </row>
     <row r="15" hidden="1">
       <c r="A15" s="53" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B15" s="49"/>
       <c r="C15" s="53" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E15" s="53"/>
       <c r="F15" s="53" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="G15" s="54"/>
     </row>
     <row r="16" hidden="1">
       <c r="A16" s="56" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="56" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="56" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="G16" s="57"/>
     </row>
     <row r="17" hidden="1">
       <c r="A17" s="53" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="53" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="53" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="G17" s="54"/>
     </row>
     <row r="18">
       <c r="A18" s="56" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="C18" s="57"/>
       <c r="D18" s="56" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="F18" s="57"/>
       <c r="G18" s="57"/>
     </row>
     <row r="19">
       <c r="A19" s="53" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E19" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="G19" s="54"/>
     </row>
     <row r="20" hidden="1">
       <c r="A20" s="56" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D20" s="56" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E20" s="56"/>
       <c r="F20" s="57"/>
@@ -28672,287 +28715,303 @@
     </row>
     <row r="21">
       <c r="A21" s="53" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B21" s="54"/>
       <c r="C21" s="53" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E21" s="53" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="G21" s="54"/>
     </row>
     <row r="22">
       <c r="A22" s="56" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B22" s="56" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C22" s="57"/>
       <c r="D22" s="56" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="G22" s="57"/>
     </row>
     <row r="23">
       <c r="A23" s="53" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="G23" s="54"/>
     </row>
     <row r="24">
       <c r="A24" s="56" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B24" s="57"/>
       <c r="C24" s="56" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="D24" s="56" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E24" s="56" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="G24" s="57"/>
     </row>
     <row r="25">
       <c r="A25" s="53" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B25" s="54"/>
       <c r="C25" s="53" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="F25" s="53" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="G25" s="54"/>
     </row>
     <row r="26">
       <c r="A26" s="56" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="56" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E26" s="56" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="G26" s="57"/>
     </row>
     <row r="27">
       <c r="A27" s="53" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B27" s="53" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="53" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E27" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F27" s="54"/>
       <c r="G27" s="54"/>
     </row>
     <row r="28">
       <c r="A28" s="56" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C28" s="57"/>
       <c r="D28" s="56" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="E28" s="56" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F28" s="57"/>
       <c r="G28" s="57"/>
     </row>
     <row r="29">
       <c r="A29" s="53" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="53" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E29" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="54"/>
     </row>
     <row r="30">
       <c r="A30" s="56" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="56" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E30" s="56" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F30" s="57"/>
       <c r="G30" s="57"/>
     </row>
     <row r="31">
       <c r="A31" s="53" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B31" s="53" t="s">
+        <v>512</v>
+      </c>
+      <c r="C31" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="D31" s="53" t="s">
         <v>508</v>
       </c>
-      <c r="C31" s="53" t="s">
-        <v>509</v>
-      </c>
-      <c r="D31" s="53" t="s">
-        <v>504</v>
-      </c>
       <c r="E31" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F31" s="54"/>
       <c r="G31" s="54"/>
     </row>
     <row r="32">
       <c r="A32" s="56" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B32" s="57"/>
       <c r="C32" s="56" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E32" s="56" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F32" s="57"/>
       <c r="G32" s="57"/>
     </row>
     <row r="33">
       <c r="A33" s="53" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
       <c r="D33" s="53" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E33" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F33" s="53" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="G33" s="54"/>
     </row>
     <row r="34">
       <c r="A34" s="56" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B34" s="57"/>
       <c r="C34" s="57"/>
       <c r="D34" s="56" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E34" s="56" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="G34" s="57"/>
     </row>
     <row r="35">
       <c r="A35" s="53" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="B35" s="54"/>
       <c r="C35" s="54"/>
       <c r="D35" s="53" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E35" s="53" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="F35" s="54"/>
       <c r="G35" s="54"/>
     </row>
     <row r="36">
-      <c r="A36" s="56"/>
+      <c r="A36" s="56" t="s">
+        <v>521</v>
+      </c>
       <c r="B36" s="57"/>
       <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
+      <c r="D36" s="56" t="s">
+        <v>508</v>
+      </c>
+      <c r="E36" s="56" t="s">
+        <v>477</v>
+      </c>
+      <c r="F36" s="56" t="s">
+        <v>522</v>
+      </c>
       <c r="G36" s="57"/>
     </row>
     <row r="37">
-      <c r="A37" s="54"/>
+      <c r="A37" s="53" t="s">
+        <v>523</v>
+      </c>
       <c r="B37" s="54"/>
       <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="D37" s="53" t="s">
+        <v>508</v>
+      </c>
+      <c r="E37" s="53" t="s">
+        <v>477</v>
+      </c>
+      <c r="F37" s="53" t="s">
+        <v>524</v>
+      </c>
       <c r="G37" s="54"/>
     </row>
     <row r="38">
@@ -37700,30 +37759,30 @@
         <v>4</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="F1" s="62" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="43" t="s">
-        <v>23</v>
+      <c r="A2" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="45"/>
-      <c r="F2" s="43" t="s">
-        <v>24</v>
+      <c r="F2" s="39" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="46" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="64"/>
@@ -37732,10 +37791,10 @@
     </row>
     <row r="4">
       <c r="A4" s="50" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="C4" s="65"/>
       <c r="D4" s="66"/>
@@ -37744,13 +37803,13 @@
     </row>
     <row r="5">
       <c r="A5" s="67" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="D5" s="64"/>
       <c r="E5" s="63"/>
@@ -45771,530 +45830,530 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="12" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="8" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="12" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="8" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="12" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="12" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="B11" s="68"/>
       <c r="C11" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="12" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="12" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="8" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="12" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D16" s="69"/>
       <c r="E16" s="17"/>
       <c r="F16" s="5" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="12" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="12" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="12" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="12" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
       <c r="F22" s="12" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="12" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="8" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="12" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="8" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="12" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="70" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="12" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="8" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="12" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="12" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="8" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="12" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="8" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="12" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="8" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="12" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="8" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="12" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
     </row>
     <row r="37">
@@ -46304,7 +46363,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="38">
@@ -46314,7 +46373,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="39">
@@ -46324,7 +46383,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="40">
@@ -46334,7 +46393,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="41">
@@ -46344,7 +46403,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="42">
@@ -46354,7 +46413,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="43">
@@ -46364,7 +46423,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="44">
@@ -46374,7 +46433,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="45">
@@ -46384,7 +46443,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="46">
@@ -46394,7 +46453,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="47">
@@ -46404,7 +46463,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="48">
@@ -46414,7 +46473,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="49">
@@ -46424,7 +46483,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
       <c r="F49" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="50">
@@ -46434,7 +46493,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="12" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
     </row>
     <row r="51">

</xml_diff>

<commit_message>
more postgres sql rows in functions.xlsx
</commit_message>
<xml_diff>
--- a/references/functions.xlsx
+++ b/references/functions.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="712">
   <si>
     <t>1. Text that needs to be replaced will be surrounded by &lt; &gt;
 2. In the case that angle brackets is part of the syntax, the following characters will be used in descending priority...&lt; &gt;
@@ -2085,14 +2085,14 @@
     <t>union_1</t>
   </si>
   <si>
-    <t>Notes:
+    <t>notes:
   1: "Does deduplicate.  Union all does not deduplicate"</t>
   </si>
   <si>
     <t>union-all_1</t>
   </si>
   <si>
-    <t>Notes:
+    <t>notes:
   1: "Does not deduplicate.  Union does deduplicate"</t>
   </si>
   <si>
@@ -2100,6 +2100,26 @@
   </si>
   <si>
     <t>UNNEST(ARRAY['2019', '2020', '2021'])    AS particip_year</t>
+  </si>
+  <si>
+    <t>privileges_1</t>
+  </si>
+  <si>
+    <t>GRANT ALL PRIVILEGES ON sources_apcd.month_to_quarter_map TO dev_apcd_group;</t>
+  </si>
+  <si>
+    <t>concat_1</t>
+  </si>
+  <si>
+    <t>concat_ws_1</t>
+  </si>
+  <si>
+    <t>SELECT
+ CONCAT_WS ('***', 'geeks ', 'for', 'geeks');</t>
+  </si>
+  <si>
+    <t>notes:
+  1: "first argument is the seperator"</t>
   </si>
   <si>
     <t>os.rename(&lt;old name&gt;, &lt;new name&gt;)</t>
@@ -2289,7 +2309,7 @@
     <t>group</t>
   </si>
   <si>
-    <t>description: "Used for logical grouping"</t>
+    <t>description: "Used for logical grouping.  Also works to capture part of a match."</t>
   </si>
   <si>
     <t>1: "/Bob|Alice/"</t>
@@ -29951,16 +29971,26 @@
       <c r="G68" s="58"/>
     </row>
     <row r="69">
-      <c r="A69" s="55"/>
-      <c r="B69" s="55"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
+      <c r="A69" s="54" t="s">
+        <v>604</v>
+      </c>
+      <c r="B69" s="50"/>
+      <c r="C69" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="D69" s="54" t="s">
+        <v>440</v>
+      </c>
+      <c r="E69" s="54" t="s">
+        <v>494</v>
+      </c>
       <c r="F69" s="55"/>
       <c r="G69" s="55"/>
     </row>
     <row r="70">
-      <c r="A70" s="58"/>
+      <c r="A70" s="57" t="s">
+        <v>606</v>
+      </c>
       <c r="B70" s="58"/>
       <c r="C70" s="58"/>
       <c r="D70" s="58"/>
@@ -29969,12 +29999,22 @@
       <c r="G70" s="58"/>
     </row>
     <row r="71">
-      <c r="A71" s="55"/>
+      <c r="A71" s="54" t="s">
+        <v>607</v>
+      </c>
       <c r="B71" s="55"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55"/>
+      <c r="C71" s="54" t="s">
+        <v>608</v>
+      </c>
+      <c r="D71" s="54" t="s">
+        <v>440</v>
+      </c>
+      <c r="E71" s="54" t="s">
+        <v>441</v>
+      </c>
+      <c r="F71" s="54" t="s">
+        <v>609</v>
+      </c>
       <c r="G71" s="55"/>
     </row>
     <row r="72">
@@ -38448,7 +38488,7 @@
         <v>135</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="C3" s="64"/>
       <c r="D3" s="65"/>
@@ -38457,10 +38497,10 @@
     </row>
     <row r="4">
       <c r="A4" s="51" t="s">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="C4" s="66"/>
       <c r="D4" s="67"/>
@@ -38469,13 +38509,13 @@
     </row>
     <row r="5">
       <c r="A5" s="68" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="D5" s="65"/>
       <c r="E5" s="64"/>
@@ -46496,324 +46536,324 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>616</v>
+        <v>622</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
       <c r="F2" s="12" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="8" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="12" t="s">
-        <v>622</v>
+        <v>628</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="8" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="12" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="12" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="12" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="12" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="12" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="12" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="B11" s="69"/>
       <c r="C11" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="12" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
     </row>
     <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="12" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="12" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="12" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="12" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="17"/>
       <c r="F16" s="5" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="12" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="12" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="12" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="12" t="s">
-        <v>660</v>
+        <v>666</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="12" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
       <c r="F22" s="12" t="s">
-        <v>666</v>
+        <v>672</v>
       </c>
     </row>
     <row r="23">
@@ -46821,205 +46861,205 @@
         <v>291</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="12" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>670</v>
+        <v>676</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="8" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="12" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="8" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="12" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="71" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="12" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="12" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="8" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="12" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="12" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="12" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="8" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="12" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="8" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="12" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="8" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="12" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="8" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="12" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
     </row>
     <row r="37">
@@ -47029,7 +47069,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="38">
@@ -47039,7 +47079,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="39">
@@ -47049,7 +47089,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="40">
@@ -47059,7 +47099,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="41">
@@ -47069,7 +47109,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="42">
@@ -47079,7 +47119,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="43">
@@ -47089,7 +47129,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="44">
@@ -47099,7 +47139,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="45">
@@ -47109,7 +47149,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="46">
@@ -47119,7 +47159,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="47">
@@ -47129,7 +47169,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="48">
@@ -47139,7 +47179,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="49">
@@ -47149,7 +47189,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
       <c r="F49" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="50">
@@ -47159,7 +47199,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="12" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="51">
@@ -54949,10 +54989,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="72" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="C1" s="74"/>
       <c r="D1" s="74"/>
@@ -54981,10 +55021,10 @@
     </row>
     <row r="2">
       <c r="A2" s="75" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>